<commit_message>
New features related to cherge
</commit_message>
<xml_diff>
--- a/Computational-chemistry-course-project/pKa/new_data.xlsx
+++ b/Computational-chemistry-course-project/pKa/new_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sashaolshanova/GramNegative-Accumulation/Computational-chemistry-course-project/pKa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AFEF0B-82BD-4F4F-9876-C67134E3ECAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1844B8-FFE4-874D-861B-2CE15B8537F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5740" yWindow="460" windowWidth="21820" windowHeight="16260" xr2:uid="{E9AE2529-900B-F645-BB64-F1A9814F71FC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>name</t>
   </si>
@@ -60,6 +60,30 @@
   </si>
   <si>
     <t>3-46</t>
+  </si>
+  <si>
+    <t>2-5</t>
+  </si>
+  <si>
+    <t>3-45</t>
+  </si>
+  <si>
+    <t>2-52</t>
+  </si>
+  <si>
+    <t>3-17</t>
+  </si>
+  <si>
+    <t>3-9</t>
+  </si>
+  <si>
+    <t>4-3</t>
+  </si>
+  <si>
+    <t>4-4</t>
+  </si>
+  <si>
+    <t>3-5</t>
   </si>
 </sst>
 </file>
@@ -108,7 +132,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.249977111117893"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -140,25 +164,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,15 +500,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE48A384-0C16-504F-94EA-52EE61A209EF}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="171" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="20.6640625" customWidth="1"/>
   </cols>
@@ -498,80 +525,148 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="8">
         <v>-3866.3890809999998</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="9">
         <v>-3865.9407510000001</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="8">
         <v>-3905.6448070000001</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="10">
         <v>-3905.2001</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="11">
         <v>-829.55175799999995</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="10">
         <v>-829.10292000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="10">
-        <v>-998.09936600000003</v>
-      </c>
-      <c r="C5" s="8">
+      <c r="B5" s="14">
         <v>-998.25520200000005</v>
       </c>
+      <c r="C5" s="15">
+        <v>-998.25520200000005</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="8">
         <v>-908.07470899999998</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="7">
         <v>-907.62341100000003</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="3">
         <v>-908.29928700000005</v>
       </c>
       <c r="C7" s="2">
-        <v>0</v>
+        <v>-907.84874000000002</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
+      <c r="A8" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2">
+        <v>-790.28488100000004</v>
+      </c>
+      <c r="C8" s="2">
+        <v>-789.83998099999997</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
+      <c r="A9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="2">
+        <v>-865.05760299999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="2">
+        <v>-923.03501200000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="2">
+        <v>-829.09526200000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2">
+        <v>-868.81282199999998</v>
+      </c>
+      <c r="C12" s="2">
+        <v>-868.362077</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2">
+        <v>-868.82882500000005</v>
+      </c>
+      <c r="C13" s="2">
+        <v>-868.37722199999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="2">
+        <v>-830.76118399999996</v>
+      </c>
+      <c r="C14" s="2">
+        <v>-830.31037500000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Feature selection based on threshold
</commit_message>
<xml_diff>
--- a/Computational-chemistry-course-project/pKa/new_data.xlsx
+++ b/Computational-chemistry-course-project/pKa/new_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sashaolshanova/GramNegative-Accumulation/Computational-chemistry-course-project/pKa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1844B8-FFE4-874D-861B-2CE15B8537F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8230557F-FC52-D949-B6A0-6280407E4641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5740" yWindow="460" windowWidth="21820" windowHeight="16260" xr2:uid="{E9AE2529-900B-F645-BB64-F1A9814F71FC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>name</t>
   </si>
@@ -47,9 +47,6 @@
     <t>2-3</t>
   </si>
   <si>
-    <t>2-46</t>
-  </si>
-  <si>
     <t>charged_pka(ΔGA-)</t>
   </si>
   <si>
@@ -65,15 +62,6 @@
     <t>2-5</t>
   </si>
   <si>
-    <t>3-45</t>
-  </si>
-  <si>
-    <t>2-52</t>
-  </si>
-  <si>
-    <t>3-17</t>
-  </si>
-  <si>
     <t>3-9</t>
   </si>
   <si>
@@ -81,9 +69,6 @@
   </si>
   <si>
     <t>4-4</t>
-  </si>
-  <si>
-    <t>3-5</t>
   </si>
 </sst>
 </file>
@@ -117,18 +102,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -164,28 +143,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE48A384-0C16-504F-94EA-52EE61A209EF}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="171" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -518,155 +491,110 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7">
+        <v>-3866.3890809999998</v>
+      </c>
+      <c r="C2" s="8">
+        <v>-3865.9407510000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7">
+        <v>-3905.6448070000001</v>
+      </c>
+      <c r="C3" s="9">
+        <v>-3905.2001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10">
+        <v>-829.55175799999995</v>
+      </c>
+      <c r="C4" s="9">
+        <v>-829.10292000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8">
-        <v>-3866.3890809999998</v>
-      </c>
-      <c r="C2" s="9">
-        <v>-3865.9407510000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="8">
-        <v>-3905.6448070000001</v>
-      </c>
-      <c r="C3" s="10">
-        <v>-3905.2001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="11">
-        <v>-829.55175799999995</v>
-      </c>
-      <c r="C4" s="10">
-        <v>-829.10292000000004</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="14">
-        <v>-998.25520200000005</v>
-      </c>
-      <c r="C5" s="15">
-        <v>-998.25520200000005</v>
+      <c r="B5" s="7">
+        <v>-908.07470899999998</v>
+      </c>
+      <c r="C5" s="6">
+        <v>-907.62341100000003</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="8">
-        <v>-908.07470899999998</v>
-      </c>
-      <c r="C6" s="7">
-        <v>-907.62341100000003</v>
+      <c r="B6" s="3">
+        <v>-908.29928700000005</v>
+      </c>
+      <c r="C6" s="2">
+        <v>-907.84874000000002</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3">
-        <v>-908.29928700000005</v>
+      <c r="B7" s="2">
+        <v>-790.28488100000004</v>
       </c>
       <c r="C7" s="2">
-        <v>-907.84874000000002</v>
+        <v>-789.83998099999997</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="2">
-        <v>-790.28488100000004</v>
+        <v>-868.81282199999998</v>
       </c>
       <c r="C8" s="2">
-        <v>-789.83998099999997</v>
+        <v>-868.362077</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="2">
+        <v>-868.82882500000005</v>
+      </c>
       <c r="C9" s="2">
-        <v>-865.05760299999997</v>
+        <v>-868.37722199999996</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="2">
+        <v>-830.76118399999996</v>
+      </c>
       <c r="C10" s="2">
-        <v>-923.03501200000005</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="2">
-        <v>-829.09526200000005</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="2">
-        <v>-868.81282199999998</v>
-      </c>
-      <c r="C12" s="2">
-        <v>-868.362077</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="2">
-        <v>-868.82882500000005</v>
-      </c>
-      <c r="C13" s="2">
-        <v>-868.37722199999996</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="2">
-        <v>-830.76118399999996</v>
-      </c>
-      <c r="C14" s="2">
         <v>-830.31037500000002</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>